<commit_message>
updates for log analytics
</commit_message>
<xml_diff>
--- a/AzureTemplateGenerator/AzureNetworkInfrastructure.xlsx
+++ b/AzureTemplateGenerator/AzureNetworkInfrastructure.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="8955" tabRatio="693" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="8955" tabRatio="693" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="SUB" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2545" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2576" uniqueCount="428">
   <si>
     <t>SUB</t>
   </si>
@@ -3577,7 +3577,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3676,8 +3676,8 @@
       <c r="H3" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>378</v>
+      <c r="I3" s="4" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -3688,10 +3688,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3705,9 +3705,10 @@
     <col min="7" max="7" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3735,8 +3736,11 @@
       <c r="I1" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>328</v>
       </c>
@@ -3762,8 +3766,11 @@
         <v>234</v>
       </c>
       <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>328</v>
       </c>
@@ -3789,6 +3796,9 @@
         <v>235</v>
       </c>
       <c r="I3" s="3"/>
+      <c r="J3" s="4" t="s">
+        <v>375</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4447,7 +4457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
@@ -4788,7 +4798,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7838,7 +7848,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="O2" sqref="O2:O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9324,10 +9334,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9338,10 +9348,10 @@
     <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9361,13 +9371,10 @@
         <v>43</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>328</v>
       </c>
@@ -9386,10 +9393,11 @@
       <c r="F2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>328</v>
       </c>
@@ -9408,10 +9416,11 @@
       <c r="F3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G3" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>328</v>
       </c>
@@ -9430,10 +9439,11 @@
       <c r="F4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>374</v>
       </c>
@@ -9452,10 +9462,11 @@
       <c r="F5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>374</v>
       </c>
@@ -9474,10 +9485,11 @@
       <c r="F6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>373</v>
       </c>
@@ -9496,10 +9508,11 @@
       <c r="F7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>373</v>
       </c>
@@ -9518,10 +9531,11 @@
       <c r="F8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G8" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>328</v>
       </c>
@@ -9540,10 +9554,11 @@
       <c r="F9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>328</v>
       </c>
@@ -9562,10 +9577,11 @@
       <c r="F10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>328</v>
       </c>
@@ -9584,10 +9600,11 @@
       <c r="F11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G11" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>374</v>
       </c>
@@ -9606,10 +9623,11 @@
       <c r="F12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G12" s="4" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>374</v>
       </c>
@@ -9628,10 +9646,11 @@
       <c r="F13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G13" s="4" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>373</v>
       </c>
@@ -9650,10 +9669,11 @@
       <c r="F14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G14" s="4" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>373</v>
       </c>
@@ -9672,8 +9692,9 @@
       <c r="F15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="G15" s="4" t="s">
+        <v>376</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10045,7 +10066,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10730,10 +10751,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10746,9 +10767,10 @@
     <col min="6" max="6" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -10773,8 +10795,11 @@
       <c r="H1" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>328</v>
       </c>
@@ -10799,8 +10824,11 @@
       <c r="H2" s="4" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>328</v>
       </c>
@@ -10825,8 +10853,11 @@
       <c r="H3" s="4" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>328</v>
       </c>
@@ -10851,8 +10882,11 @@
       <c r="H4" s="4" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>374</v>
       </c>
@@ -10877,8 +10911,11 @@
       <c r="H5" s="4" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>374</v>
       </c>
@@ -10903,8 +10940,11 @@
       <c r="H6" s="4" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>373</v>
       </c>
@@ -10929,8 +10969,11 @@
       <c r="H7" s="4" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>373</v>
       </c>
@@ -10955,8 +10998,11 @@
       <c r="H8" s="4" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>328</v>
       </c>
@@ -10981,8 +11027,11 @@
       <c r="H9" s="3" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>328</v>
       </c>
@@ -11007,8 +11056,11 @@
       <c r="H10" s="3" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>328</v>
       </c>
@@ -11033,8 +11085,11 @@
       <c r="H11" s="3" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>374</v>
       </c>
@@ -11059,8 +11114,11 @@
       <c r="H12" s="3" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="4" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>374</v>
       </c>
@@ -11085,8 +11143,11 @@
       <c r="H13" s="3" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="4" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>373</v>
       </c>
@@ -11111,8 +11172,11 @@
       <c r="H14" s="3" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="4" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>373</v>
       </c>
@@ -11136,6 +11200,9 @@
       </c>
       <c r="H15" s="3" t="s">
         <v>233</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LAW updates and FullDeploy updates
</commit_message>
<xml_diff>
--- a/AzureTemplateGenerator/AzureNetworkInfrastructure.xlsx
+++ b/AzureTemplateGenerator/AzureNetworkInfrastructure.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="8955" tabRatio="693" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="8955" tabRatio="693" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="SUB" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2576" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2576" uniqueCount="426">
   <si>
     <t>SUB</t>
   </si>
@@ -1320,13 +1320,7 @@
     <t>DNPRD-CAEA-EXTWORKLOAD-RT</t>
   </si>
   <si>
-    <t>0b251b66-c41d-4ea3-925e-b6ce6b64f970</t>
-  </si>
-  <si>
-    <t>f5963e61-482e-47a2-a706-b31c08078662</t>
-  </si>
-  <si>
-    <t>f7154194-75eb-4c75-9b8e-78fb73c783d5</t>
+    <t>xxxxxxxx-xxxx-xxxx-xxxx-xxxxxxxxxxxx</t>
   </si>
 </sst>
 </file>
@@ -1779,7 +1773,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1809,7 +1803,7 @@
         <v>373</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1817,7 +1811,7 @@
         <v>374</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -3577,7 +3571,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3690,8 +3684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4182,7 +4176,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4354,7 +4350,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4798,7 +4794,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5115,7 +5111,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5217,7 +5213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V110"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -7848,7 +7844,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O31"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8664,7 +8660,7 @@
       <c r="N17" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="O17" s="3" t="s">
+      <c r="O17" s="4" t="s">
         <v>375</v>
       </c>
     </row>
@@ -8711,7 +8707,7 @@
       <c r="N18" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="O18" s="3" t="s">
+      <c r="O18" s="4" t="s">
         <v>375</v>
       </c>
     </row>
@@ -8758,7 +8754,7 @@
       <c r="N19" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="O19" s="3" t="s">
+      <c r="O19" s="4" t="s">
         <v>375</v>
       </c>
     </row>
@@ -8805,7 +8801,7 @@
       <c r="N20" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="O20" s="3" t="s">
+      <c r="O20" s="4" t="s">
         <v>375</v>
       </c>
     </row>
@@ -8852,7 +8848,7 @@
       <c r="N21" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="O21" s="3" t="s">
+      <c r="O21" s="4" t="s">
         <v>375</v>
       </c>
     </row>
@@ -8899,7 +8895,7 @@
       <c r="N22" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="O22" s="3" t="s">
+      <c r="O22" s="4" t="s">
         <v>375</v>
       </c>
     </row>
@@ -8946,7 +8942,7 @@
       <c r="N23" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="O23" s="3" t="s">
+      <c r="O23" s="4" t="s">
         <v>375</v>
       </c>
     </row>
@@ -8993,7 +8989,7 @@
       <c r="N24" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="O24" s="3" t="s">
+      <c r="O24" s="4" t="s">
         <v>376</v>
       </c>
     </row>
@@ -9040,7 +9036,7 @@
       <c r="N25" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="O25" s="3" t="s">
+      <c r="O25" s="4" t="s">
         <v>376</v>
       </c>
     </row>
@@ -9087,7 +9083,7 @@
       <c r="N26" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="O26" s="3" t="s">
+      <c r="O26" s="4" t="s">
         <v>376</v>
       </c>
     </row>
@@ -9134,7 +9130,7 @@
       <c r="N27" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="O27" s="3" t="s">
+      <c r="O27" s="4" t="s">
         <v>376</v>
       </c>
     </row>
@@ -9181,7 +9177,7 @@
       <c r="N28" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="O28" s="3" t="s">
+      <c r="O28" s="4" t="s">
         <v>377</v>
       </c>
     </row>
@@ -9228,7 +9224,7 @@
       <c r="N29" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="O29" s="3" t="s">
+      <c r="O29" s="4" t="s">
         <v>377</v>
       </c>
     </row>
@@ -9275,7 +9271,7 @@
       <c r="N30" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="O30" s="3" t="s">
+      <c r="O30" s="4" t="s">
         <v>377</v>
       </c>
     </row>
@@ -9322,7 +9318,7 @@
       <c r="N31" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="O31" s="3" t="s">
+      <c r="O31" s="4" t="s">
         <v>377</v>
       </c>
     </row>
@@ -9337,7 +9333,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adjusted LAW settings on NSGs
</commit_message>
<xml_diff>
--- a/AzureTemplateGenerator/AzureNetworkInfrastructure.xlsx
+++ b/AzureTemplateGenerator/AzureNetworkInfrastructure.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="8955" tabRatio="693" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="8955" tabRatio="693"/>
   </bookViews>
   <sheets>
     <sheet name="SUB" sheetId="2" r:id="rId1"/>
@@ -1772,8 +1772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5213,7 +5213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -9333,7 +9333,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9459,7 +9459,7 @@
         <v>42</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -9482,7 +9482,7 @@
         <v>42</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -9505,7 +9505,7 @@
         <v>42</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -9528,7 +9528,7 @@
         <v>42</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -9703,7 +9703,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9778,7 +9778,7 @@
         <v>92</v>
       </c>
       <c r="E2" s="21">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="F2" s="20" t="s">
         <v>93</v>
@@ -9819,7 +9819,7 @@
         <v>92</v>
       </c>
       <c r="E3" s="21">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F3" s="20" t="s">
         <v>93</v>
@@ -9860,7 +9860,7 @@
         <v>92</v>
       </c>
       <c r="E4" s="21">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="F4" s="20" t="s">
         <v>93</v>

</xml_diff>

<commit_message>
fixed VNET settings. (incorrect LAW reference)
</commit_message>
<xml_diff>
--- a/AzureTemplateGenerator/AzureNetworkInfrastructure.xlsx
+++ b/AzureTemplateGenerator/AzureNetworkInfrastructure.xlsx
@@ -1320,7 +1320,7 @@
     <t>DNPRD-CAEA-EXTWORKLOAD-RT</t>
   </si>
   <si>
-    <t>xxxxxxxx-xxxx-xxxx-xxxx-xxxxxxxxxxxx</t>
+    <t>xxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxx</t>
   </si>
 </sst>
 </file>
@@ -1773,7 +1773,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4177,7 +4177,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10750,7 +10750,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10908,7 +10908,7 @@
         <v>223</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -10937,7 +10937,7 @@
         <v>224</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -10966,7 +10966,7 @@
         <v>225</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -10995,7 +10995,7 @@
         <v>226</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated VNET template generation to properly handle GATEWAYS and FIREWALLS
</commit_message>
<xml_diff>
--- a/AzureTemplateGenerator/AzureNetworkInfrastructure.xlsx
+++ b/AzureTemplateGenerator/AzureNetworkInfrastructure.xlsx
@@ -1320,7 +1320,7 @@
     <t>DNPRD-CAEA-EXTWORKLOAD-RT</t>
   </si>
   <si>
-    <t>xxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxx</t>
+    <t>xxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxx</t>
   </si>
 </sst>
 </file>
@@ -1773,7 +1773,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11212,7 +11212,7 @@
   <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>